<commit_message>
Reordered subroutines and updated the excel file some
</commit_message>
<xml_diff>
--- a/Subroutines.xlsx
+++ b/Subroutines.xlsx
@@ -654,15 +654,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:XFD61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="33.21875" customWidth="1"/>
   </cols>
@@ -820,183 +820,183 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>30</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C39" t="s">
         <v>42</v>
       </c>
     </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>66</v>
-      </c>
       <c r="C41" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>67</v>
-      </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C45" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>68</v>
+      </c>
       <c r="C46" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>69</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>70</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>72</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved init, changed maze icon to tetris icon, started working on menu system.
</commit_message>
<xml_diff>
--- a/Subroutines.xlsx
+++ b/Subroutines.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>lsr2-7</t>
   </si>
@@ -111,27 +111,6 @@
     <t>generateRandom4BitValue</t>
   </si>
   <si>
-    <t>logos</t>
-  </si>
-  <si>
-    <t>drawSnakeLogo</t>
-  </si>
-  <si>
-    <t>drawMazeLogo</t>
-  </si>
-  <si>
-    <t>drawAsteroidLogo</t>
-  </si>
-  <si>
-    <t>drawTimerLogo</t>
-  </si>
-  <si>
-    <t>drawRandomLogo</t>
-  </si>
-  <si>
-    <t>drawJoystickLogo</t>
-  </si>
-  <si>
     <t>draw</t>
   </si>
   <si>
@@ -289,6 +268,30 @@
   </si>
   <si>
     <t>timer</t>
+  </si>
+  <si>
+    <t>programSelectMenu</t>
+  </si>
+  <si>
+    <t>icons</t>
+  </si>
+  <si>
+    <t>drawSnakeIcon</t>
+  </si>
+  <si>
+    <t>drawMazeIcon</t>
+  </si>
+  <si>
+    <t>drawAsteroidIcon</t>
+  </si>
+  <si>
+    <t>drawTimerIcon</t>
+  </si>
+  <si>
+    <t>drawRandomIcon</t>
+  </si>
+  <si>
+    <t>drawJoystickIcon</t>
   </si>
 </sst>
 </file>
@@ -656,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,7 +701,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
@@ -706,7 +709,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
@@ -714,7 +717,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>11</v>
@@ -788,7 +791,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>23</v>
@@ -796,7 +799,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>24</v>
@@ -804,7 +807,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>25</v>
@@ -812,7 +815,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>27</v>
@@ -820,184 +823,189 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C46" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>28</v>
-      </c>
       <c r="C49" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
         <v>30</v>
       </c>
     </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>69</v>
-      </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>70</v>
-      </c>
       <c r="C57" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C60" t="s">
-        <v>64</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>72</v>
-      </c>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1024,13 +1032,13 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1043,7 +1051,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1051,64 +1059,64 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added subroutines to excel and small fix in the Tetris game.
</commit_message>
<xml_diff>
--- a/Subroutines.xlsx
+++ b/Subroutines.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Subroutines" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="105">
   <si>
     <t>lsr2-7</t>
   </si>
@@ -87,9 +87,6 @@
     <t>initializeFlashFood</t>
   </si>
   <si>
-    <t>mazeGame</t>
-  </si>
-  <si>
     <t>asteroids</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t>drawSnakeIcon</t>
   </si>
   <si>
-    <t>drawMazeIcon</t>
-  </si>
-  <si>
     <t>drawAsteroidIcon</t>
   </si>
   <si>
@@ -292,6 +286,51 @@
   </si>
   <si>
     <t>drawJoystickIcon</t>
+  </si>
+  <si>
+    <t>tetrisGame</t>
+  </si>
+  <si>
+    <t>initializeTetris</t>
+  </si>
+  <si>
+    <t>tetrisStartAnimation</t>
+  </si>
+  <si>
+    <t>tetrisEndAnimation</t>
+  </si>
+  <si>
+    <t>tetrisClearFullRows</t>
+  </si>
+  <si>
+    <t>tetrisUpdate</t>
+  </si>
+  <si>
+    <t>tetrisJoyStickUpdate</t>
+  </si>
+  <si>
+    <t>tetrisNextBlock</t>
+  </si>
+  <si>
+    <t>tetrisCheckCollision</t>
+  </si>
+  <si>
+    <t>drawTetrisBlock</t>
+  </si>
+  <si>
+    <t>clearTetrisBlock</t>
+  </si>
+  <si>
+    <t>drawTetrisIcon</t>
+  </si>
+  <si>
+    <t>isPixelSet (Not game specific)</t>
+  </si>
+  <si>
+    <t>isPixelClear (Not game specific)</t>
+  </si>
+  <si>
+    <t>PLACEHOLDER</t>
   </si>
 </sst>
 </file>
@@ -307,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,13 +361,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="135"/>
@@ -353,9 +416,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,33 +724,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="33.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -691,325 +758,411 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C22" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="5" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C37" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C38" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
+    <row r="40" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C43" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>28</v>
-      </c>
-      <c r="C48" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>63</v>
-      </c>
-      <c r="C56" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
         <v>65</v>
       </c>
-      <c r="C61" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C64" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1021,102 +1174,102 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>82</v>
       </c>
-      <c r="B6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1130,7 +1283,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Impemented new menu system. Finishing touches to Tetris.
</commit_message>
<xml_diff>
--- a/Subroutines.xlsx
+++ b/Subroutines.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Subroutines" sheetId="1" r:id="rId1"/>
     <sheet name="Macros" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="109">
   <si>
     <t>lsr2-7</t>
   </si>
@@ -273,9 +273,6 @@
     <t>drawSnakeIcon</t>
   </si>
   <si>
-    <t>drawAsteroidIcon</t>
-  </si>
-  <si>
     <t>drawTimerIcon</t>
   </si>
   <si>
@@ -321,16 +318,31 @@
     <t>drawTetrisIcon</t>
   </si>
   <si>
-    <t>isPixelSet (Not game specific)</t>
-  </si>
-  <si>
-    <t>isPixelClear (Not game specific)</t>
-  </si>
-  <si>
     <t>PLACEHOLDER</t>
   </si>
   <si>
     <t xml:space="preserve"> 'Tetris'</t>
+  </si>
+  <si>
+    <t>isPixelSet</t>
+  </si>
+  <si>
+    <t>isPixelClear</t>
+  </si>
+  <si>
+    <t>drawAsteroidsIcon</t>
+  </si>
+  <si>
+    <t>drawFillBoardIcon</t>
+  </si>
+  <si>
+    <t>dsfg</t>
+  </si>
+  <si>
+    <t>hsfg</t>
+  </si>
+  <si>
+    <t>outOfBoundsWriteMatrix</t>
   </si>
 </sst>
 </file>
@@ -438,7 +450,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -724,20 +736,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -749,8 +761,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -758,12 +770,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -774,7 +786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>49</v>
       </c>
@@ -782,7 +794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>50</v>
       </c>
@@ -790,185 +802,190 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C22" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C22" s="7" t="s">
+    <row r="23" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C23" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C23" s="7" t="s">
+    <row r="24" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C24" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C24" s="7" t="s">
+    <row r="25" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C25" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C25" s="7" t="s">
+    <row r="26" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C26" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C26" s="7" t="s">
+    <row r="27" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C27" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C27" s="7" t="s">
+    <row r="28" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C28" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C28" s="7" t="s">
+    <row r="29" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C29" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C29" s="7" t="s">
+    <row r="30" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C30" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C30" s="7" t="s">
+    <row r="31" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C31" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C31" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C32" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B34" s="3" t="s">
+    <row r="32" spans="2:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B32" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="C32" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C33" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C34" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C35" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C36" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C37" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C38" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C39" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B40" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C40" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B40" s="3" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C41" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -976,7 +993,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>83</v>
       </c>
@@ -984,174 +1001,215 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
+    <row r="48" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
+    <row r="49" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>30</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
+    <row r="53" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
+    <row r="54" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="56" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>58</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C61" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
+    <row r="62" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C64" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C60" t="s">
+    <row r="67" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="68" spans="1:3" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>59</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C69" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="70" spans="1:3" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>27</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C71" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
+    <row r="72" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="73" spans="1:3" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>60</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C74" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C68" t="s">
+    <row r="75" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C69" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C70" t="s">
+    <row r="77" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="78" spans="1:3" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>61</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C79" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C73" t="s">
+    <row r="80" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C74" t="s">
+    <row r="81" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C75" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>63</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C84" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C78" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C79" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C80" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C81" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1169,13 +1227,13 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1183,8 +1241,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -1192,12 +1250,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -1205,7 +1263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -1213,22 +1271,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -1236,17 +1294,17 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1254,7 +1312,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1262,7 +1320,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>77</v>
       </c>
@@ -1278,7 +1336,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Started working on asteroids.
</commit_message>
<xml_diff>
--- a/Subroutines.xlsx
+++ b/Subroutines.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
   <si>
     <t>lsr2-7</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>outOfBoundsWriteMatrix</t>
+  </si>
+  <si>
+    <t>spawnAsteroid</t>
   </si>
 </sst>
 </file>
@@ -738,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +939,7 @@
     </row>
     <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C33" s="9" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -1170,12 +1173,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Added generic code for the ship and bullets (spawn, move remove, etc.)
</commit_message>
<xml_diff>
--- a/Subroutines.xlsx
+++ b/Subroutines.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
   <si>
     <t>lsr2-7</t>
   </si>
@@ -358,6 +358,30 @@
   </si>
   <si>
     <t>Categories / Programs</t>
+  </si>
+  <si>
+    <t>moveShip</t>
+  </si>
+  <si>
+    <t>drawShip</t>
+  </si>
+  <si>
+    <t>createBullet</t>
+  </si>
+  <si>
+    <t>moveBullets</t>
+  </si>
+  <si>
+    <t>drawBullets</t>
+  </si>
+  <si>
+    <t>flashBullets</t>
+  </si>
+  <si>
+    <t>removeBullet</t>
+  </si>
+  <si>
+    <t>removeDeadBullets</t>
   </si>
 </sst>
 </file>
@@ -752,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B89"/>
+  <dimension ref="A1:B97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,6 +968,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
       <c r="B33" s="8" t="s">
         <v>112</v>
       </c>
@@ -955,264 +980,304 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B35" s="8" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B36" s="8" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B39" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B48" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B49" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>55</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B51" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>81</v>
-      </c>
-      <c r="B45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="B53" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B60" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>56</v>
-      </c>
       <c r="B62" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B64" s="3" t="s">
-        <v>99</v>
+      <c r="B64" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B65" s="3" t="s">
-        <v>100</v>
+      <c r="B65" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>25</v>
-      </c>
-      <c r="B72" t="s">
-        <v>26</v>
+      <c r="B72" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
-        <v>27</v>
+      <c r="B73" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>58</v>
-      </c>
       <c r="B75" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>57</v>
+      </c>
       <c r="B78" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="B80" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B82" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>58</v>
+      </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>61</v>
-      </c>
       <c r="B85" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B87" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>59</v>
+      </c>
       <c r="B88" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>61</v>
+      </c>
+      <c r="B93" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added an explosion animation to asteroids.
</commit_message>
<xml_diff>
--- a/Subroutines.xlsx
+++ b/Subroutines.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="125">
   <si>
     <t>lsr2-7</t>
   </si>
@@ -327,21 +327,9 @@
     <t>drawFillBoardIcon</t>
   </si>
   <si>
-    <t>dsfg</t>
-  </si>
-  <si>
-    <t>hsfg</t>
-  </si>
-  <si>
-    <t>outOfBoundsWriteMatrix</t>
-  </si>
-  <si>
     <t>spawnAsteroid</t>
   </si>
   <si>
-    <t>valueToDirection8</t>
-  </si>
-  <si>
     <t>removeAsteroid</t>
   </si>
   <si>
@@ -360,6 +348,9 @@
     <t>Categories / Programs</t>
   </si>
   <si>
+    <t>indexToDirection8</t>
+  </si>
+  <si>
     <t>moveShip</t>
   </si>
   <si>
@@ -382,6 +373,24 @@
   </si>
   <si>
     <t>removeDeadBullets</t>
+  </si>
+  <si>
+    <t>drawAsteroidsExplosionAnimationFrame</t>
+  </si>
+  <si>
+    <t>asteroidsEndAnimation</t>
+  </si>
+  <si>
+    <t>direction8ToIndex</t>
+  </si>
+  <si>
+    <t>drawOutOfBoundsWriteMatrix</t>
+  </si>
+  <si>
+    <t>drawOutOfBoundsReadMatrix</t>
+  </si>
+  <si>
+    <t>drawCrossMatrix</t>
   </si>
 </sst>
 </file>
@@ -459,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="135"/>
@@ -467,6 +476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -776,21 +786,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.21875" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="37.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -812,472 +822,492 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+    <row r="23" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B24" s="6" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B27" s="6" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B28" s="6" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B29" s="6" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B30" s="6" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B31" s="6" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
+    <row r="35" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B36" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="8" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B34" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B35" s="8" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B36" s="8" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B37" s="8" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B38" s="8" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B39" s="8" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B40" s="8" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B41" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B42" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B43" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B44" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B45" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B46" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B47" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
+    <row r="53" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B54" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
+    <row r="55" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B56" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>55</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B58" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>81</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B60" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B57" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B58" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B59" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>28</v>
-      </c>
-      <c r="B61" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
       <c r="B68" t="s">
-        <v>104</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>56</v>
-      </c>
       <c r="B70" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
-        <v>35</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B72" s="3" t="s">
-        <v>99</v>
+      <c r="B72" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B73" s="3" t="s">
-        <v>100</v>
+      <c r="B73" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>56</v>
+      </c>
+      <c r="B76" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B76" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>57</v>
-      </c>
-      <c r="B78" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>25</v>
-      </c>
-      <c r="B80" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>57</v>
+      </c>
+      <c r="B84" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>58</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B89" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B84" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B85" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B86" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>59</v>
-      </c>
-      <c r="B88" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B89" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
-        <v>53</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>61</v>
-      </c>
       <c r="B93" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>59</v>
+      </c>
+      <c r="B96" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>61</v>
+      </c>
+      <c r="B101" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B95" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B96" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B97" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Tetris start and end animations. Updated Subourines.
</commit_message>
<xml_diff>
--- a/Subroutines.xlsx
+++ b/Subroutines.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Subroutines" sheetId="1" r:id="rId1"/>
     <sheet name="Macros" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="126">
   <si>
     <t>lsr2-7</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>drawCrossMatrix</t>
+  </si>
+  <si>
+    <t>initializeTetrisBlocks</t>
   </si>
 </sst>
 </file>
@@ -786,19 +789,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.21875" customWidth="1"/>
-    <col min="2" max="2" width="37.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>109</v>
       </c>
@@ -807,8 +810,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:2" s="3" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -816,12 +819,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>46</v>
       </c>
@@ -829,10 +832,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>47</v>
       </c>
@@ -840,10 +843,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>48</v>
       </c>
@@ -851,74 +854,74 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>98</v>
       </c>
@@ -926,388 +929,406 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B26" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="7" t="s">
+    <row r="27" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B27" s="7" t="s">
+    <row r="28" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B28" s="7" t="s">
+    <row r="29" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B29" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B29" s="7" t="s">
+    <row r="30" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B30" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B30" s="7" t="s">
+    <row r="31" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B31" s="7" t="s">
+    <row r="32" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B32" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B32" s="7" t="s">
+    <row r="33" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B33" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="7" t="s">
+    <row r="34" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B34" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B34" s="7" t="s">
+    <row r="35" spans="1:2" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
+    <row r="36" spans="1:2" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B37" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="9" t="s">
+    <row r="38" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B38" s="9" t="s">
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B39" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B39" s="9" t="s">
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B40" s="9" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B40" s="9" t="s">
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B41" s="9" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B41" s="9" t="s">
+    <row r="42" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B42" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B42" s="9" t="s">
+    <row r="43" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B43" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B43" s="9" t="s">
+    <row r="44" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B44" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B44" s="9" t="s">
+    <row r="45" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B45" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B45" s="9" t="s">
+    <row r="46" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B46" s="9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B46" s="9" t="s">
+    <row r="47" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B47" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B47" s="9" t="s">
+    <row r="48" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B48" s="9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B48" s="9" t="s">
+    <row r="49" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B49" s="9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B49" s="9" t="s">
+    <row r="50" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B50" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B50" s="9" t="s">
+    <row r="51" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B51" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B51" s="9" t="s">
+    <row r="52" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B52" s="9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B52" s="9" t="s">
+    <row r="53" spans="1:2" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A53"/>
+      <c r="B53" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="10" t="s">
+    <row r="54" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="1:2" s="3" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B55" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="11" t="s">
+    <row r="56" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B57" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="58" spans="1:2" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>55</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="60" spans="1:2" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>81</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B61" t="s">
+    <row r="62" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B62" t="s">
+    <row r="63" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B63" t="s">
+    <row r="64" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
+    <row r="65" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
+    <row r="66" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B66" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="68" spans="1:2" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>28</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B69" t="s">
+    <row r="70" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B70" t="s">
+    <row r="71" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
+    <row r="72" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
+    <row r="73" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
+    <row r="74" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="76" spans="1:2" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>56</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
+    <row r="78" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B78" s="3" t="s">
+    <row r="79" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B79" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B79" s="3" t="s">
+    <row r="80" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B80" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B80" t="s">
+    <row r="81" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B81" t="s">
+    <row r="82" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B82" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="84" spans="1:2" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>57</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="86" spans="1:2" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>25</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B87" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>58</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B90" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B91" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B92" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B93" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B94" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>59</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B97" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B98" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B99" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>61</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B102" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B103" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B104" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B105" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1325,13 +1346,13 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1339,8 +1360,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1348,12 +1369,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1361,7 +1382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -1369,22 +1390,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -1392,17 +1413,17 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1410,7 +1431,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1418,7 +1439,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>75</v>
       </c>
@@ -1434,7 +1455,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>